<commit_message>
svm L1 L2 Separately
</commit_message>
<xml_diff>
--- a/result_v2(8.23).xlsx
+++ b/result_v2(8.23).xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20338"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kara\Documents\MRs-of-linear-models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kara\Documents\MR-of-ML\linear models\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BED2EF-37E8-4B5B-821B-9B4943954A5E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12240"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="150">
   <si>
     <t>MR1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -486,13 +487,28 @@
   </si>
   <si>
     <t>w_curr = w -step_size-0.031047126290037783 * gradient</t>
+  </si>
+  <si>
+    <t>b_curr =b+0.12729193727342922 - step_size * gradient_b</t>
+  </si>
+  <si>
+    <t>b_curr = b -step_size+0.5539443047647777 * gradient_b</t>
+  </si>
+  <si>
+    <t>b_curr = b - step_size *gradient_b+0.5293549766700935</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> w = (1 -gamma-0.008003863215121487) * w_curr + gamma * w_prev</t>
+  </si>
+  <si>
+    <t>w = (1 - gamma) *w_curr-0.9117207568581369 + gamma * w_prev</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -852,23 +868,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J49" workbookViewId="0">
-      <selection activeCell="M59" sqref="M59"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="J65" sqref="J65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="10" width="9" style="1"/>
-    <col min="11" max="12" width="12.5" style="1" customWidth="1"/>
-    <col min="13" max="13" width="73.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.125" style="1" customWidth="1"/>
+    <col min="11" max="12" width="12.44140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="73.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.109375" style="1" customWidth="1"/>
     <col min="15" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -906,7 +922,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -948,7 +964,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
@@ -990,7 +1006,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>0.76</v>
       </c>
@@ -1026,7 +1042,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1068,7 +1084,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -1110,7 +1126,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -1152,7 +1168,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -1191,7 +1207,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -1236,7 +1252,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -1278,7 +1294,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -1320,7 +1336,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
@@ -1362,7 +1378,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>0</v>
       </c>
@@ -1398,7 +1414,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
@@ -1440,7 +1456,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
@@ -1482,7 +1498,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
@@ -1521,7 +1537,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
@@ -1560,7 +1576,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>33</v>
       </c>
@@ -1599,7 +1615,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
@@ -1638,7 +1654,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>35</v>
       </c>
@@ -1677,7 +1693,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -1716,7 +1732,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>37</v>
       </c>
@@ -1755,7 +1771,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>38</v>
       </c>
@@ -1794,7 +1810,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>39</v>
       </c>
@@ -1833,7 +1849,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>40</v>
       </c>
@@ -1872,7 +1888,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>41</v>
       </c>
@@ -1911,7 +1927,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>42</v>
       </c>
@@ -1950,7 +1966,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>43</v>
       </c>
@@ -1989,7 +2005,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>44</v>
       </c>
@@ -2028,7 +2044,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>45</v>
       </c>
@@ -2067,7 +2083,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>46</v>
       </c>
@@ -2106,7 +2122,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>47</v>
       </c>
@@ -2145,7 +2161,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>48</v>
       </c>
@@ -2184,7 +2200,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>49</v>
       </c>
@@ -2223,7 +2239,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>50</v>
       </c>
@@ -2262,7 +2278,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>51</v>
       </c>
@@ -2301,7 +2317,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>52</v>
       </c>
@@ -2340,7 +2356,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>53</v>
       </c>
@@ -2379,7 +2395,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>54</v>
       </c>
@@ -2424,7 +2440,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>55</v>
       </c>
@@ -2463,7 +2479,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>56</v>
       </c>
@@ -2505,7 +2521,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>57</v>
       </c>
@@ -2544,7 +2560,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>58</v>
       </c>
@@ -2586,7 +2602,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>59</v>
       </c>
@@ -2625,7 +2641,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>60</v>
       </c>
@@ -2664,7 +2680,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>61</v>
       </c>
@@ -2703,7 +2719,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>62</v>
       </c>
@@ -2742,7 +2758,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>63</v>
       </c>
@@ -2789,7 +2805,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>64</v>
       </c>
@@ -2828,7 +2844,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>65</v>
       </c>
@@ -2867,7 +2883,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>66</v>
       </c>
@@ -2906,7 +2922,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>67</v>
       </c>
@@ -2945,7 +2961,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>68</v>
       </c>
@@ -2984,7 +3000,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>137</v>
       </c>
@@ -3023,7 +3039,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>125</v>
       </c>
@@ -3062,7 +3078,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>126</v>
       </c>
@@ -3101,7 +3117,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>127</v>
       </c>
@@ -3140,7 +3156,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>128</v>
       </c>
@@ -3179,103 +3195,280 @@
         <v>142</v>
       </c>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>129</v>
       </c>
       <c r="B59" s="1">
-        <v>0</v>
+        <v>0.44</v>
       </c>
       <c r="C59" s="1">
         <v>0</v>
       </c>
       <c r="D59" s="1">
-        <v>0</v>
+        <v>0.54</v>
       </c>
       <c r="E59" s="1">
-        <v>0</v>
+        <v>0.54</v>
       </c>
       <c r="F59" s="1">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="G59" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="H59" s="1">
+        <v>0.68</v>
+      </c>
+      <c r="I59" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="J59" s="1">
         <v>0.06</v>
       </c>
-      <c r="H59" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="I59" s="1">
-        <v>0</v>
-      </c>
-      <c r="J59" s="1">
-        <v>0</v>
-      </c>
       <c r="K59" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M59" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>130</v>
       </c>
+      <c r="B60" s="1">
+        <v>0</v>
+      </c>
+      <c r="C60" s="1">
+        <v>0</v>
+      </c>
+      <c r="D60" s="1">
+        <v>0.78</v>
+      </c>
+      <c r="E60" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="F60" s="1">
+        <v>0</v>
+      </c>
+      <c r="G60" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="H60" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="I60" s="1">
+        <v>0</v>
+      </c>
+      <c r="J60" s="1">
+        <v>0.12</v>
+      </c>
       <c r="K60" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M60" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>131</v>
       </c>
+      <c r="B61" s="1">
+        <v>0</v>
+      </c>
+      <c r="C61" s="1">
+        <v>0</v>
+      </c>
+      <c r="D61" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="E61" s="1">
+        <v>0.64</v>
+      </c>
+      <c r="F61" s="1">
+        <v>0</v>
+      </c>
+      <c r="G61" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="H61" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="I61" s="1">
+        <v>0</v>
+      </c>
+      <c r="J61" s="1">
+        <v>0.08</v>
+      </c>
       <c r="K61" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13">
+        <v>2</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="B62" s="1">
+        <v>0</v>
+      </c>
+      <c r="C62" s="1">
+        <v>0</v>
+      </c>
+      <c r="D62" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="E62" s="1">
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="G62" s="1">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="H62" s="1">
+        <v>1</v>
+      </c>
+      <c r="I62" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="J62" s="1">
+        <v>0.62</v>
+      </c>
       <c r="K62" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13">
+        <v>5</v>
+      </c>
+      <c r="M62" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>133</v>
       </c>
+      <c r="B63" s="1">
+        <v>0</v>
+      </c>
+      <c r="C63" s="1">
+        <v>0</v>
+      </c>
+      <c r="D63" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="E63" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="F63" s="1">
+        <v>0</v>
+      </c>
+      <c r="G63" s="1">
+        <v>0</v>
+      </c>
+      <c r="H63" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="I63" s="1">
+        <v>0.26</v>
+      </c>
+      <c r="J63" s="1">
+        <v>0</v>
+      </c>
       <c r="K63" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13">
+        <v>4</v>
+      </c>
+      <c r="M63" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>134</v>
       </c>
+      <c r="B64" s="1">
+        <v>0</v>
+      </c>
+      <c r="C64" s="1">
+        <v>0</v>
+      </c>
+      <c r="D64" s="1">
+        <v>0</v>
+      </c>
+      <c r="E64" s="1">
+        <v>0</v>
+      </c>
+      <c r="F64" s="1">
+        <v>0</v>
+      </c>
+      <c r="G64" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="H64" s="1">
+        <v>0</v>
+      </c>
+      <c r="I64" s="1">
+        <v>0</v>
+      </c>
+      <c r="J64" s="1">
+        <v>0</v>
+      </c>
       <c r="K64" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:11">
+      <c r="M64" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>135</v>
       </c>
+      <c r="B65" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="C65" s="1">
+        <v>0</v>
+      </c>
+      <c r="D65" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="E65" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="F65" s="1">
+        <v>0</v>
+      </c>
+      <c r="G65" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="H65" s="1">
+        <v>0.52</v>
+      </c>
+      <c r="I65" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="J65" s="1">
+        <v>0.04</v>
+      </c>
       <c r="K65" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11">
+        <v>4</v>
+      </c>
+      <c r="M65" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>136</v>
       </c>
@@ -3284,13 +3477,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>112</v>
       </c>
       <c r="B68" s="1">
         <f>COUNTIF(B1:B66,"&gt;=0.1")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C68" s="1">
         <f t="shared" ref="C68:J68" si="2">COUNTIF(C1:C66,"&gt;=0.1")</f>
@@ -3298,31 +3491,31 @@
       </c>
       <c r="D68" s="1">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E68" s="1">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F68" s="1">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G68" s="1">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H68" s="1">
         <f>COUNTIF(H1:H66,"&gt;=0.1")+4</f>
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="I68" s="1">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J68" s="1">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new mutants and results
</commit_message>
<xml_diff>
--- a/result_v2(8.23).xlsx
+++ b/result_v2(8.23).xlsx
@@ -16,7 +16,6 @@
     <sheet name="LR_NM" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="212">
   <si>
     <t>MR1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -581,6 +580,122 @@
   </si>
   <si>
     <t>alpha = (np.dot(r0.T,r0+0.07382007600389018)/np.maximum(1e-12, np.dot(p.T, Ap)))</t>
+  </si>
+  <si>
+    <t>alpha = (np.dot(r0.T, r0)/np.maximum(1e-12, np.dot(p.T,1.3424042829341503*Ap)))</t>
+  </si>
+  <si>
+    <t>alpha = (np.dot(r0.T, r0)/np.maximum(1e-12, np.dot(p.T,Ap-0.26867576382653763)))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x = x - p * alpha</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x = x + p / alpha</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> x =1.0686657575987044*x + p * alpha</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x =x-0.06134264954484758 + p * alpha</t>
+  </si>
+  <si>
+    <t>x = x +0.8237859279218015*p * alpha</t>
+  </si>
+  <si>
+    <t>x = x +p-0.08944143512793183 * alpha</t>
+  </si>
+  <si>
+    <t>BUG50</t>
+  </si>
+  <si>
+    <t>x = x + p *0.8459892000798297*alpha</t>
+  </si>
+  <si>
+    <t>x = x + p *alpha+0.07980283863323827</t>
+  </si>
+  <si>
+    <t>r = r0 + Ap * alpha</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r =0.9718283556459395*r0 - Ap * alpha</t>
+  </si>
+  <si>
+    <t>r =r0+1.1383210111305517 - Ap * alpha</t>
+  </si>
+  <si>
+    <t>r = r0 -0.8641826721522685*Ap * alpha</t>
+  </si>
+  <si>
+    <t>t</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r = r0 - Ap *1.1883390665047944*alpha</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r = r0 - Ap *alpha-0.7202844785947524</t>
+  </si>
+  <si>
+    <t>z = np.dot(0.9011171832984325*M, r)</t>
+  </si>
+  <si>
+    <t>z = np.dot(M-0.4334766445036269, r)</t>
+  </si>
+  <si>
+    <t>z = np.dot(M,1.0724758988155971*r)</t>
+  </si>
+  <si>
+    <t>z = np.dot(M,r-1.035435004138049)</t>
+  </si>
+  <si>
+    <t>beta = (np.dot(r.T, z)/np.dot(r0.T,0.641199787365405*z0))</t>
+  </si>
+  <si>
+    <t>beta = (np.dot(r.T,1.2736857613189454*z)/np.dot(r0.T, z0))</t>
+  </si>
+  <si>
+    <t>beta = (np.dot(r.T, z)/np.dot(r0.T,z0-0.8382966093257396))</t>
+  </si>
+  <si>
+    <t>p = z - beta * p</t>
+  </si>
+  <si>
+    <t>p = z + beta / p</t>
+  </si>
+  <si>
+    <t>p = 0.8982623348917906 * z + beta * p</t>
+  </si>
+  <si>
+    <t>p =z-0.49235833017824787 + beta * p</t>
+  </si>
+  <si>
+    <t>p = z +0.9860904506527102*beta * p</t>
+  </si>
+  <si>
+    <t>BUG41</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p = z + beta + 0.595177658219508 * p</t>
+  </si>
+  <si>
+    <t>p = z + beta *p+0.2955578302051637</t>
+  </si>
+  <si>
+    <t>return .5 * (1 + np.tanh(0.6725395318396448 * x))</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> grad = + X.T * (y - self.p1(X * beta))</t>
+  </si>
+  <si>
+    <t>grad = - X.T * (y + self.p1(X * beta)) mutate104</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -657,7 +772,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -677,6 +792,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -978,20 +1096,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
     </row>
     <row r="2" spans="1:14">
       <c r="B2" s="1" t="s">
@@ -3910,944 +4028,1985 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M46"/>
+  <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="H32" workbookViewId="0">
+      <selection activeCell="M48" sqref="M48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="10" width="6.625" customWidth="1"/>
-    <col min="11" max="11" width="12.5" customWidth="1"/>
-    <col min="12" max="12" width="10.75" customWidth="1"/>
-    <col min="13" max="13" width="70.125" customWidth="1"/>
-    <col min="14" max="14" width="9" customWidth="1"/>
+    <col min="1" max="1" width="7" style="7" customWidth="1"/>
+    <col min="2" max="10" width="6.625" style="7" customWidth="1"/>
+    <col min="11" max="11" width="12.5" style="7" customWidth="1"/>
+    <col min="12" max="12" width="10.75" style="7" customWidth="1"/>
+    <col min="13" max="13" width="70.125" style="7" customWidth="1"/>
+    <col min="14" max="14" width="9" style="7" customWidth="1"/>
+    <col min="15" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="1"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="7" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="B3" s="7">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
         <v>0.92</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="7">
         <v>0.66</v>
       </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1">
+      <c r="F3" s="7">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
+      <c r="H3" s="7">
         <v>1</v>
       </c>
-      <c r="I3" s="1">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1">
+      <c r="I3" s="7">
+        <v>0</v>
+      </c>
+      <c r="J3" s="7">
         <v>0.08</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="7">
         <f>COUNTIF(B3:J3,"&gt;=0.1")</f>
         <v>3</v>
       </c>
-      <c r="L3" s="1"/>
-      <c r="M3" t="s">
+      <c r="M3" s="7" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="B4" s="1">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0</v>
-      </c>
-      <c r="K4" s="1">
-        <f t="shared" ref="K4:K30" si="0">COUNTIF(B4:J4,"&gt;=0.1")</f>
-        <v>0</v>
-      </c>
-      <c r="L4" s="1"/>
-      <c r="M4" t="s">
+      <c r="B4" s="7">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7">
+        <v>0</v>
+      </c>
+      <c r="G4" s="7">
+        <v>0</v>
+      </c>
+      <c r="H4" s="7">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7">
+        <v>0</v>
+      </c>
+      <c r="J4" s="7">
+        <v>0</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" ref="K4:K52" si="0">COUNTIF(B4:J4,"&gt;=0.1")</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="7" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="B5" s="7">
+        <v>0</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0</v>
+      </c>
+      <c r="D5" s="7">
         <v>0.5</v>
       </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1">
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0</v>
+      </c>
+      <c r="H5" s="7">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7">
+        <v>0</v>
+      </c>
+      <c r="J5" s="7">
         <v>0.2</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="7">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="L5" s="1"/>
-      <c r="M5" t="s">
+      <c r="M5" s="7" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1">
-        <v>0</v>
-      </c>
-      <c r="J6" s="1">
-        <v>0</v>
-      </c>
-      <c r="K6" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L6" s="1"/>
-      <c r="M6" t="s">
+      <c r="B6" s="7">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7">
+        <v>0</v>
+      </c>
+      <c r="J6" s="7">
+        <v>0</v>
+      </c>
+      <c r="K6" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M6" s="7" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="1">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1">
+      <c r="B7" s="7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7">
         <v>0.08</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="7">
         <v>0.02</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="7">
         <v>0.02</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="7">
         <v>0.04</v>
       </c>
-      <c r="I7" s="1">
-        <v>0</v>
-      </c>
-      <c r="J7" s="1">
-        <v>0</v>
-      </c>
-      <c r="K7" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L7" s="1"/>
-      <c r="M7" t="s">
+      <c r="I7" s="7">
+        <v>0</v>
+      </c>
+      <c r="J7" s="7">
+        <v>0</v>
+      </c>
+      <c r="K7" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M7" s="7" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1">
-        <v>0</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1">
-        <v>0</v>
-      </c>
-      <c r="J8" s="1">
-        <v>0</v>
-      </c>
-      <c r="K8" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L8" s="1"/>
-      <c r="M8" t="s">
+      <c r="B8" s="7">
+        <v>0</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0</v>
+      </c>
+      <c r="H8" s="7">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7">
+        <v>0</v>
+      </c>
+      <c r="J8" s="7">
+        <v>0</v>
+      </c>
+      <c r="K8" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="7" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="7">
         <v>0.04</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="7">
         <v>0.02</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="7">
         <v>0.16</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="7">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="7">
         <v>0.08</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="7">
         <v>0.12</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="7">
         <v>0.34</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="7">
         <v>0.02</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="7">
         <v>0.12</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="7">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="L9" s="1"/>
-      <c r="M9" t="s">
+      <c r="M9" s="7" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="1">
-        <v>0</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1">
+      <c r="B10" s="7">
+        <v>0</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0</v>
+      </c>
+      <c r="D10" s="7">
         <f>-D100</f>
         <v>0</v>
       </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0</v>
-      </c>
-      <c r="H10" s="1">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1">
-        <v>0</v>
-      </c>
-      <c r="J10" s="1">
-        <v>0</v>
-      </c>
-      <c r="K10" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L10" s="1"/>
-      <c r="M10" t="s">
+      <c r="E10" s="7">
+        <v>0</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0</v>
+      </c>
+      <c r="G10" s="7">
+        <v>0</v>
+      </c>
+      <c r="H10" s="7">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7">
+        <v>0</v>
+      </c>
+      <c r="J10" s="7">
+        <v>0</v>
+      </c>
+      <c r="K10" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="7" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="B11" s="1">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1">
+      <c r="B11" s="7">
+        <v>0</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0</v>
+      </c>
+      <c r="D11" s="7">
         <f>-D101</f>
         <v>0</v>
       </c>
-      <c r="E11" s="1">
-        <v>0</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1">
-        <v>0</v>
-      </c>
-      <c r="J11" s="1">
-        <v>0</v>
-      </c>
-      <c r="K11" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L11" s="1"/>
-      <c r="M11" t="s">
+      <c r="E11" s="7">
+        <v>0</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0</v>
+      </c>
+      <c r="G11" s="7">
+        <v>0</v>
+      </c>
+      <c r="H11" s="7">
+        <v>0</v>
+      </c>
+      <c r="I11" s="7">
+        <v>0</v>
+      </c>
+      <c r="J11" s="7">
+        <v>0</v>
+      </c>
+      <c r="K11" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="7" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="7">
         <v>0.04</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="7">
         <v>0.02</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="7">
         <v>0.84</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="7">
         <v>0.84</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="7">
         <v>0.08</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="7">
         <v>0.44</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="7">
         <v>1</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="7">
         <v>0.26</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12" s="7">
         <v>0.22</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12" s="7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="L12" s="1"/>
-      <c r="M12" t="s">
+      <c r="M12" s="7" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="1">
-        <v>0</v>
-      </c>
-      <c r="C13" s="1">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0</v>
-      </c>
-      <c r="E13" s="1">
-        <v>0</v>
-      </c>
-      <c r="F13" s="1">
-        <v>0</v>
-      </c>
-      <c r="G13" s="1">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1">
-        <v>0</v>
-      </c>
-      <c r="I13" s="1">
-        <v>0</v>
-      </c>
-      <c r="J13" s="1">
-        <v>0</v>
-      </c>
-      <c r="K13" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L13" s="1"/>
-      <c r="M13" t="s">
+      <c r="B13" s="7">
+        <v>0</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0</v>
+      </c>
+      <c r="F13" s="7">
+        <v>0</v>
+      </c>
+      <c r="G13" s="7">
+        <v>0</v>
+      </c>
+      <c r="H13" s="7">
+        <v>0</v>
+      </c>
+      <c r="I13" s="7">
+        <v>0</v>
+      </c>
+      <c r="J13" s="7">
+        <v>0</v>
+      </c>
+      <c r="K13" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="7" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="1">
-        <v>0</v>
-      </c>
-      <c r="C14" s="1">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1">
+      <c r="B14" s="7">
+        <v>0</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0</v>
+      </c>
+      <c r="D14" s="7">
         <v>0.04</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="7">
         <v>0.04</v>
       </c>
-      <c r="F14" s="1">
-        <v>0</v>
-      </c>
-      <c r="G14" s="1">
-        <v>0</v>
-      </c>
-      <c r="H14" s="1">
+      <c r="F14" s="7">
+        <v>0</v>
+      </c>
+      <c r="G14" s="7">
+        <v>0</v>
+      </c>
+      <c r="H14" s="7">
         <v>0.4</v>
       </c>
-      <c r="I14" s="1">
-        <v>0</v>
-      </c>
-      <c r="J14" s="1">
-        <v>0</v>
-      </c>
-      <c r="K14" s="1">
+      <c r="I14" s="7">
+        <v>0</v>
+      </c>
+      <c r="J14" s="7">
+        <v>0</v>
+      </c>
+      <c r="K14" s="7">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="L14" s="1"/>
-      <c r="M14" t="s">
+      <c r="M14" s="7" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L15" s="1"/>
+      <c r="B15" s="7">
+        <v>0</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0</v>
+      </c>
+      <c r="D15" s="7">
+        <v>0</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0</v>
+      </c>
+      <c r="F15" s="7">
+        <v>0</v>
+      </c>
+      <c r="G15" s="7">
+        <v>0</v>
+      </c>
+      <c r="H15" s="7">
+        <v>0</v>
+      </c>
+      <c r="I15" s="7">
+        <v>0</v>
+      </c>
+      <c r="J15" s="7">
+        <v>0</v>
+      </c>
+      <c r="K15" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L16" s="1"/>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="A17" s="1" t="s">
+      <c r="B16" s="7">
+        <v>0</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="D16" s="7">
+        <v>1</v>
+      </c>
+      <c r="E16" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="F16" s="7">
+        <v>0.32</v>
+      </c>
+      <c r="G16" s="7">
+        <v>0.82</v>
+      </c>
+      <c r="H16" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="I16" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="J16" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="K16" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="M16" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L17" s="1"/>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="A18" s="1" t="s">
+      <c r="B17" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D17" s="7">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E17" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="F17" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="G17" s="7">
+        <v>0.94</v>
+      </c>
+      <c r="H17" s="7">
+        <v>0.84</v>
+      </c>
+      <c r="I17" s="7">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="J17" s="7">
+        <v>0.48</v>
+      </c>
+      <c r="K17" s="7">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L18" s="1"/>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="A19" s="1" t="s">
+      <c r="B18" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="C18" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="D18" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="E18" s="7">
+        <v>0.34</v>
+      </c>
+      <c r="F18" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="G18" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="H18" s="7">
+        <v>0.92</v>
+      </c>
+      <c r="I18" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="J18" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="K18" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M18" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L19" s="1"/>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="A20" s="1" t="s">
+      <c r="B19" s="7">
+        <v>0</v>
+      </c>
+      <c r="C19" s="7">
+        <v>0</v>
+      </c>
+      <c r="D19" s="7">
+        <v>0</v>
+      </c>
+      <c r="E19" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="F19" s="7">
+        <v>0</v>
+      </c>
+      <c r="G19" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="H19" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="I19" s="7">
+        <v>0</v>
+      </c>
+      <c r="J19" s="7">
+        <v>0</v>
+      </c>
+      <c r="K19" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M19" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L20" s="1"/>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="A21" s="1" t="s">
+      <c r="B20" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="C20" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="D20" s="7">
+        <v>0.98</v>
+      </c>
+      <c r="E20" s="7">
+        <v>0.92</v>
+      </c>
+      <c r="F20" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="G20" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="H20" s="7">
+        <v>1</v>
+      </c>
+      <c r="I20" s="7">
+        <v>0</v>
+      </c>
+      <c r="J20" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="K20" s="7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M20" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L21" s="1"/>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="A22" s="1" t="s">
+      <c r="B21" s="7">
+        <v>0</v>
+      </c>
+      <c r="C21" s="7">
+        <v>0</v>
+      </c>
+      <c r="D21" s="7">
+        <v>0</v>
+      </c>
+      <c r="E21" s="7">
+        <v>0</v>
+      </c>
+      <c r="F21" s="7">
+        <v>0</v>
+      </c>
+      <c r="G21" s="7">
+        <v>0</v>
+      </c>
+      <c r="H21" s="7">
+        <v>0</v>
+      </c>
+      <c r="I21" s="7">
+        <v>0</v>
+      </c>
+      <c r="J21" s="7">
+        <v>0</v>
+      </c>
+      <c r="K21" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L22" s="1"/>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="A23" s="1" t="s">
+      <c r="B22" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="C22" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="D22" s="7">
+        <v>1</v>
+      </c>
+      <c r="E22" s="7">
+        <v>0.98</v>
+      </c>
+      <c r="F22" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="G22" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="H22" s="7">
+        <v>0.96</v>
+      </c>
+      <c r="I22" s="7">
+        <v>0.48</v>
+      </c>
+      <c r="J22" s="7">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="K22" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="M22" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L23" s="1"/>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="1" t="s">
+      <c r="B23" s="7">
+        <v>0</v>
+      </c>
+      <c r="C23" s="7">
+        <v>0</v>
+      </c>
+      <c r="D23" s="7">
+        <v>0</v>
+      </c>
+      <c r="E23" s="7">
+        <v>0</v>
+      </c>
+      <c r="F23" s="7">
+        <v>0</v>
+      </c>
+      <c r="G23" s="7">
+        <v>0</v>
+      </c>
+      <c r="H23" s="7">
+        <v>0</v>
+      </c>
+      <c r="I23" s="7">
+        <v>0</v>
+      </c>
+      <c r="J23" s="7">
+        <v>0</v>
+      </c>
+      <c r="K23" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M23" s="7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L24" s="1"/>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25" s="1" t="s">
+      <c r="B24" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="C24" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="D24" s="7">
+        <v>0.96</v>
+      </c>
+      <c r="E24" s="7">
+        <v>0.92</v>
+      </c>
+      <c r="F24" s="7">
+        <v>0.18</v>
+      </c>
+      <c r="G24" s="7">
+        <v>0.82</v>
+      </c>
+      <c r="H24" s="7">
+        <v>0.98</v>
+      </c>
+      <c r="I24" s="7">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J24" s="7">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K24" s="7">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="M24" s="7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L25" s="1"/>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="1" t="s">
+      <c r="B25" s="7">
+        <v>0</v>
+      </c>
+      <c r="C25" s="7">
+        <v>0</v>
+      </c>
+      <c r="D25" s="7">
+        <v>0</v>
+      </c>
+      <c r="E25" s="7">
+        <v>0.78</v>
+      </c>
+      <c r="F25" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="G25" s="7">
+        <v>0.26</v>
+      </c>
+      <c r="H25" s="7">
+        <v>1</v>
+      </c>
+      <c r="I25" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="J25" s="7">
+        <v>0.16</v>
+      </c>
+      <c r="K25" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="M25" s="7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L26" s="1"/>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="A27" s="1" t="s">
+      <c r="B26" s="7">
+        <v>0</v>
+      </c>
+      <c r="C26" s="7">
+        <v>0</v>
+      </c>
+      <c r="D26" s="7">
+        <v>0</v>
+      </c>
+      <c r="E26" s="7">
+        <v>0.72</v>
+      </c>
+      <c r="F26" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="G26" s="7">
+        <v>0.22</v>
+      </c>
+      <c r="H26" s="7">
+        <v>0.72</v>
+      </c>
+      <c r="I26" s="7">
+        <v>0.16</v>
+      </c>
+      <c r="J26" s="7">
+        <v>0.18</v>
+      </c>
+      <c r="K26" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="M26" s="7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L27" s="1"/>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="A28" s="1" t="s">
+      <c r="B27" s="7">
+        <v>0</v>
+      </c>
+      <c r="C27" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="D27" s="7">
+        <v>0.96</v>
+      </c>
+      <c r="E27" s="7">
+        <v>0.72</v>
+      </c>
+      <c r="F27" s="7">
+        <v>0</v>
+      </c>
+      <c r="G27" s="7">
+        <v>0.54</v>
+      </c>
+      <c r="H27" s="7">
+        <v>1</v>
+      </c>
+      <c r="I27" s="7">
+        <v>0</v>
+      </c>
+      <c r="J27" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="K27" s="7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M27" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L28" s="1"/>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="1" t="s">
+      <c r="B28" s="7">
+        <v>0</v>
+      </c>
+      <c r="C28" s="7">
+        <v>0</v>
+      </c>
+      <c r="D28" s="7">
+        <v>0</v>
+      </c>
+      <c r="E28" s="7">
+        <v>0</v>
+      </c>
+      <c r="F28" s="7">
+        <v>0</v>
+      </c>
+      <c r="G28" s="7">
+        <v>0</v>
+      </c>
+      <c r="H28" s="7">
+        <v>0</v>
+      </c>
+      <c r="I28" s="7">
+        <v>0</v>
+      </c>
+      <c r="J28" s="7">
+        <v>0</v>
+      </c>
+      <c r="K28" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M28" s="7" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L29" s="1"/>
-    </row>
-    <row r="30" spans="1:12">
-      <c r="A30" s="1" t="s">
+      <c r="B29" s="7">
+        <v>0</v>
+      </c>
+      <c r="C29" s="7">
+        <v>0</v>
+      </c>
+      <c r="D29" s="7">
+        <v>0</v>
+      </c>
+      <c r="E29" s="7">
+        <v>0.66</v>
+      </c>
+      <c r="F29" s="7">
+        <v>0</v>
+      </c>
+      <c r="G29" s="7">
+        <v>0.46</v>
+      </c>
+      <c r="H29" s="7">
+        <v>1</v>
+      </c>
+      <c r="I29" s="7">
+        <v>0.36</v>
+      </c>
+      <c r="J29" s="7">
+        <v>0.34</v>
+      </c>
+      <c r="K29" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="M29" s="7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L30" s="1"/>
-    </row>
-    <row r="45" spans="1:10">
-      <c r="A45" s="1" t="s">
+      <c r="B30" s="7">
+        <v>0</v>
+      </c>
+      <c r="C30" s="7">
+        <v>0</v>
+      </c>
+      <c r="D30" s="7">
+        <v>0</v>
+      </c>
+      <c r="E30" s="7">
+        <v>0.66</v>
+      </c>
+      <c r="F30" s="7">
+        <v>0</v>
+      </c>
+      <c r="G30" s="7">
+        <v>0.46</v>
+      </c>
+      <c r="H30" s="7">
+        <v>1</v>
+      </c>
+      <c r="I30" s="7">
+        <v>0.36</v>
+      </c>
+      <c r="J30" s="7">
+        <v>0.34</v>
+      </c>
+      <c r="K30" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="M30" s="7" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="7">
+        <v>0</v>
+      </c>
+      <c r="C31" s="7">
+        <v>0</v>
+      </c>
+      <c r="D31" s="7">
+        <v>0</v>
+      </c>
+      <c r="E31" s="7">
+        <v>0.66</v>
+      </c>
+      <c r="F31" s="7">
+        <v>0</v>
+      </c>
+      <c r="G31" s="7">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="H31" s="7">
+        <v>1</v>
+      </c>
+      <c r="I31" s="7">
+        <v>0.42</v>
+      </c>
+      <c r="J31" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="K31" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="M31" s="7" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="C32" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="D32" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="E32" s="7">
+        <v>0.46</v>
+      </c>
+      <c r="F32" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="G32" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="H32" s="7">
+        <v>0.86</v>
+      </c>
+      <c r="I32" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="J32" s="7">
+        <v>0</v>
+      </c>
+      <c r="K32" s="7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M32" s="7" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="7">
+        <v>0</v>
+      </c>
+      <c r="C33" s="7">
+        <v>0</v>
+      </c>
+      <c r="D33" s="7">
+        <v>0</v>
+      </c>
+      <c r="E33" s="7">
+        <v>0</v>
+      </c>
+      <c r="F33" s="7">
+        <v>0</v>
+      </c>
+      <c r="G33" s="7">
+        <v>0</v>
+      </c>
+      <c r="H33" s="7">
+        <v>0</v>
+      </c>
+      <c r="I33" s="7">
+        <v>0</v>
+      </c>
+      <c r="J33" s="7">
+        <v>0</v>
+      </c>
+      <c r="K33" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M33" s="7" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="C34" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="D34" s="7">
+        <v>0.94</v>
+      </c>
+      <c r="E34" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="F34" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="G34" s="7">
+        <v>0.68</v>
+      </c>
+      <c r="H34" s="7">
+        <v>0.96</v>
+      </c>
+      <c r="I34" s="7">
+        <v>0.26</v>
+      </c>
+      <c r="J34" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="K34" s="7">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="M34" s="7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="7">
+        <v>0</v>
+      </c>
+      <c r="C35" s="7">
+        <v>0</v>
+      </c>
+      <c r="D35" s="7">
+        <v>0</v>
+      </c>
+      <c r="E35" s="7">
+        <v>0</v>
+      </c>
+      <c r="F35" s="7">
+        <v>0</v>
+      </c>
+      <c r="G35" s="7">
+        <v>0</v>
+      </c>
+      <c r="H35" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="I35" s="7">
+        <v>0</v>
+      </c>
+      <c r="J35" s="7">
+        <v>0</v>
+      </c>
+      <c r="K35" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M35" s="7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" s="7">
+        <v>0</v>
+      </c>
+      <c r="C36" s="7">
+        <v>0</v>
+      </c>
+      <c r="D36" s="7">
+        <v>0</v>
+      </c>
+      <c r="E36" s="7">
+        <v>0</v>
+      </c>
+      <c r="F36" s="7">
+        <v>0</v>
+      </c>
+      <c r="G36" s="7">
+        <v>0</v>
+      </c>
+      <c r="H36" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="I36" s="7">
+        <v>0</v>
+      </c>
+      <c r="J36" s="7">
+        <v>0</v>
+      </c>
+      <c r="K36" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M36" s="7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="7">
+        <v>0</v>
+      </c>
+      <c r="C37" s="7">
+        <v>0</v>
+      </c>
+      <c r="D37" s="7">
+        <v>0</v>
+      </c>
+      <c r="E37" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="F37" s="7">
+        <v>0</v>
+      </c>
+      <c r="G37" s="7">
+        <v>0</v>
+      </c>
+      <c r="H37" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="I37" s="7">
+        <v>0</v>
+      </c>
+      <c r="J37" s="7">
+        <v>0</v>
+      </c>
+      <c r="K37" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M37" s="7" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="7">
+        <v>0</v>
+      </c>
+      <c r="C38" s="7">
+        <v>0</v>
+      </c>
+      <c r="D38" s="7">
+        <v>0</v>
+      </c>
+      <c r="E38" s="7">
+        <v>0</v>
+      </c>
+      <c r="F38" s="7">
+        <v>0</v>
+      </c>
+      <c r="G38" s="7">
+        <v>0</v>
+      </c>
+      <c r="H38" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="I38" s="7">
+        <v>0</v>
+      </c>
+      <c r="J38" s="7">
+        <v>0</v>
+      </c>
+      <c r="K38" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M38" s="7" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" s="7">
+        <v>0</v>
+      </c>
+      <c r="C39" s="7">
+        <v>0</v>
+      </c>
+      <c r="D39" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="E39" s="7">
+        <v>0</v>
+      </c>
+      <c r="F39" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="G39" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="H39" s="7">
+        <v>0.92</v>
+      </c>
+      <c r="I39" s="7">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J39" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="K39" s="7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M39" s="7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" s="7">
+        <v>0</v>
+      </c>
+      <c r="C40" s="7">
+        <v>0</v>
+      </c>
+      <c r="D40" s="7">
+        <v>0</v>
+      </c>
+      <c r="E40" s="7">
+        <v>0.84</v>
+      </c>
+      <c r="F40" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="G40" s="7">
+        <v>0.52</v>
+      </c>
+      <c r="H40" s="7">
+        <v>1</v>
+      </c>
+      <c r="I40" s="7">
+        <v>0.34</v>
+      </c>
+      <c r="J40" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="K40" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="M40" s="7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B41" s="7">
+        <v>0</v>
+      </c>
+      <c r="C41" s="7">
+        <v>0</v>
+      </c>
+      <c r="D41" s="7">
+        <v>0.98</v>
+      </c>
+      <c r="E41" s="7">
+        <v>0.96</v>
+      </c>
+      <c r="F41" s="7">
+        <v>0.26</v>
+      </c>
+      <c r="G41" s="7">
+        <v>0.88</v>
+      </c>
+      <c r="H41" s="7">
+        <v>1</v>
+      </c>
+      <c r="I41" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="J41" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="K41" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="M41" s="7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" s="7">
+        <v>0</v>
+      </c>
+      <c r="C42" s="7">
+        <v>0</v>
+      </c>
+      <c r="D42" s="7">
+        <v>0</v>
+      </c>
+      <c r="E42" s="7">
+        <v>0</v>
+      </c>
+      <c r="F42" s="7">
+        <v>0</v>
+      </c>
+      <c r="G42" s="7">
+        <v>0</v>
+      </c>
+      <c r="H42" s="7">
+        <v>0</v>
+      </c>
+      <c r="I42" s="7">
+        <v>0</v>
+      </c>
+      <c r="J42" s="7">
+        <v>0</v>
+      </c>
+      <c r="K42" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M42" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="B43" s="7">
+        <v>1</v>
+      </c>
+      <c r="C43" s="7">
+        <v>0.96</v>
+      </c>
+      <c r="D43" s="7">
+        <v>0.78</v>
+      </c>
+      <c r="E43" s="7">
+        <v>0.76</v>
+      </c>
+      <c r="F43" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="G43" s="7">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="H43" s="7">
+        <v>1</v>
+      </c>
+      <c r="I43" s="7">
+        <v>0.18</v>
+      </c>
+      <c r="J43" s="7">
+        <v>0.22</v>
+      </c>
+      <c r="K43" s="7">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="M43" s="7" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B44" s="7">
+        <v>0</v>
+      </c>
+      <c r="C44" s="7">
+        <v>0</v>
+      </c>
+      <c r="D44" s="7">
+        <v>0.94</v>
+      </c>
+      <c r="E44" s="7">
+        <v>0.96</v>
+      </c>
+      <c r="F44" s="7">
+        <v>0.38</v>
+      </c>
+      <c r="G44" s="7">
+        <v>0.96</v>
+      </c>
+      <c r="H44" s="7">
+        <v>1</v>
+      </c>
+      <c r="I44" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="J44" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="K44" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="M44" s="7" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B45" s="7">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C45" s="7">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D45" s="7">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E45" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="F45" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="G45" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="H45" s="7">
+        <v>0.84</v>
+      </c>
+      <c r="I45" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="J45" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="K45" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="M45" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B46" s="7">
+        <v>0</v>
+      </c>
+      <c r="C46" s="7">
+        <v>0</v>
+      </c>
+      <c r="D46" s="7">
+        <v>0</v>
+      </c>
+      <c r="E46" s="7">
+        <v>0</v>
+      </c>
+      <c r="F46" s="7">
+        <v>0</v>
+      </c>
+      <c r="G46" s="7">
+        <v>0</v>
+      </c>
+      <c r="H46" s="7">
+        <v>0</v>
+      </c>
+      <c r="I46" s="7">
+        <v>0</v>
+      </c>
+      <c r="J46" s="7">
+        <v>0</v>
+      </c>
+      <c r="K46" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M46" s="7" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B47" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="C47" s="7">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D47" s="7">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E47" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="F47" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="G47" s="7">
+        <v>0.94</v>
+      </c>
+      <c r="H47" s="7">
+        <v>0.84</v>
+      </c>
+      <c r="I47" s="7">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="J47" s="7">
+        <v>0.48</v>
+      </c>
+      <c r="K47" s="7">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="M47" s="7" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="K48" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M48" s="7" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="K49" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="K50" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="A51" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="K51" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="K52" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="B45" s="1">
-        <f>COUNTIF(B1:B30,"&gt;=0.1")</f>
-        <v>0</v>
-      </c>
-      <c r="C45" s="1">
-        <f t="shared" ref="C45:J45" si="1">COUNTIF(C1:C30,"&gt;=0.1")</f>
-        <v>0</v>
-      </c>
-      <c r="D45" s="1">
+      <c r="B59" s="7">
+        <f>COUNTIF(B1:B56,"&gt;=0.1")</f>
+        <v>4</v>
+      </c>
+      <c r="C59" s="7">
+        <f t="shared" ref="C59:J59" si="1">COUNTIF(C1:C56,"&gt;=0.1")</f>
+        <v>5</v>
+      </c>
+      <c r="D59" s="7">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="E45" s="1">
+        <v>17</v>
+      </c>
+      <c r="E59" s="7">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="F45" s="1">
+        <v>23</v>
+      </c>
+      <c r="F59" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G45" s="1">
+        <v>7</v>
+      </c>
+      <c r="G59" s="7">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="H45" s="1">
+        <v>20</v>
+      </c>
+      <c r="H59" s="7">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="I45" s="1">
+        <v>26</v>
+      </c>
+      <c r="I59" s="7">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J45" s="1">
+        <v>14</v>
+      </c>
+      <c r="J59" s="7">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10">
-      <c r="A46" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="B46" s="1">
-        <f xml:space="preserve"> B45/COUNT(B1:B30)</f>
-        <v>0</v>
-      </c>
-      <c r="C46" s="1">
-        <f t="shared" ref="C46:J46" si="2" xml:space="preserve"> C45/COUNT(C1:C30)</f>
-        <v>0</v>
-      </c>
-      <c r="D46" s="1">
+      <c r="B60" s="7">
+        <f xml:space="preserve"> B59/COUNT(B1:B56)</f>
+        <v>8.8888888888888892E-2</v>
+      </c>
+      <c r="C60" s="7">
+        <f t="shared" ref="C60:J60" si="2" xml:space="preserve"> C59/COUNT(C1:C56)</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D60" s="7">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="E46" s="1">
+        <v>0.37777777777777777</v>
+      </c>
+      <c r="E60" s="7">
         <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-      <c r="F46" s="1">
+        <v>0.51111111111111107</v>
+      </c>
+      <c r="F60" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G46" s="1">
+        <v>0.15555555555555556</v>
+      </c>
+      <c r="G60" s="7">
         <f t="shared" si="2"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="H46" s="1">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="H60" s="7">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="I46" s="1">
+        <v>0.57777777777777772</v>
+      </c>
+      <c r="I60" s="7">
         <f t="shared" si="2"/>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="J46" s="1">
+        <v>0.31111111111111112</v>
+      </c>
+      <c r="J60" s="7">
         <f t="shared" si="2"/>
-        <v>0.25</v>
+        <v>0.35555555555555557</v>
       </c>
     </row>
   </sheetData>
@@ -4856,5 +6015,6 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>